<commit_message>
tested loading - still pre-beta
</commit_message>
<xml_diff>
--- a/hospitalActivity/hospital1/Jun97PatientActivity.xlsx
+++ b/hospitalActivity/hospital1/Jun97PatientActivity.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/82cfe7acc6d68563/Documents/github/Clinical-Costing/hospitalActivity/hospital1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="915" documentId="8_{DD708ED2-34D1-49EE-AD2C-BABD70908E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7132F6D9-CFEF-4220-8B53-853AC2634027}"/>
+  <xr:revisionPtr revIDLastSave="926" documentId="8_{DD708ED2-34D1-49EE-AD2C-BABD70908E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEC8064D-993C-48B1-AA80-9BF8CFEF1490}"/>
   <bookViews>
-    <workbookView xWindow="28605" yWindow="-15480" windowWidth="28035" windowHeight="13035" firstSheet="3" activeTab="3" xr2:uid="{E28251DD-307F-42E2-A9BA-4292566B016A}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="11" xr2:uid="{E28251DD-307F-42E2-A9BA-4292566B016A}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="6" r:id="rId1"/>
@@ -2128,7 +2128,8 @@
   <dimension ref="A1:O614"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A614"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -31020,7 +31021,8 @@
   <dimension ref="A1:A609"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -34085,8 +34087,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FDCBE12-D5B4-460E-AB8F-A0BAE8EFEBB9}">
   <dimension ref="A1:A612"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P10" sqref="P10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -37167,7 +37170,8 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -37202,7 +37206,8 @@
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -37250,8 +37255,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1141B60C-502C-443A-B2A3-E4F8915D2C08}">
   <dimension ref="A1:U405"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -63617,7 +63623,8 @@
   <dimension ref="A1:A361"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P9" sqref="P9"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -65443,7 +65450,8 @@
   <dimension ref="A1:A373"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -67328,8 +67336,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E74AC53-01B5-4A68-BDAA-FB7300F848B6}">
   <dimension ref="A1:G473"/>
   <sheetViews>
-    <sheetView topLeftCell="A451" workbookViewId="0">
-      <selection activeCell="J466" sqref="J466"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -78235,7 +78244,8 @@
   <dimension ref="A1:K147"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -83410,7 +83420,8 @@
   <dimension ref="A1:K376"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>

<commit_message>
Added build_events - still pre-Beta
</commit_message>
<xml_diff>
--- a/hospitalActivity/hospital1/Jun97PatientActivity.xlsx
+++ b/hospitalActivity/hospital1/Jun97PatientActivity.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="926" documentId="8_{DD708ED2-34D1-49EE-AD2C-BABD70908E07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EEC8064D-993C-48B1-AA80-9BF8CFEF1490}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="6" activeTab="11" xr2:uid="{E28251DD-307F-42E2-A9BA-4292566B016A}"/>
+    <workbookView xWindow="28590" yWindow="-15285" windowWidth="29010" windowHeight="14235" firstSheet="3" activeTab="3" xr2:uid="{E28251DD-307F-42E2-A9BA-4292566B016A}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="6" r:id="rId1"/>
@@ -34087,7 +34087,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3FDCBE12-D5B4-460E-AB8F-A0BAE8EFEBB9}">
   <dimension ref="A1:A612"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="P10" sqref="P10"/>
     </sheetView>
@@ -37255,9 +37255,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1141B60C-502C-443A-B2A3-E4F8915D2C08}">
   <dimension ref="A1:U405"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -63624,7 +63624,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>

</xml_diff>